<commit_message>
added several elections to xlsx file
</commit_message>
<xml_diff>
--- a/bundestag_full.xlsx
+++ b/bundestag_full.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/default/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/default/course_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D85273-F855-1E41-8C20-85A2F3C1D588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF80277-9C6C-374E-AF3A-6E5FF326983D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>Year</t>
   </si>
@@ -152,6 +152,63 @@
   </si>
   <si>
     <t>55.578</t>
+  </si>
+  <si>
+    <t>18.488.668</t>
+  </si>
+  <si>
+    <t>14.167.561</t>
+  </si>
+  <si>
+    <t>4.315.080</t>
+  </si>
+  <si>
+    <t>4.110.355</t>
+  </si>
+  <si>
+    <t>3.538.815</t>
+  </si>
+  <si>
+    <t>PDS</t>
+  </si>
+  <si>
+    <t>1.916.702</t>
+  </si>
+  <si>
+    <t>20.181.269</t>
+  </si>
+  <si>
+    <t>14.004.908</t>
+  </si>
+  <si>
+    <t>3.324.480</t>
+  </si>
+  <si>
+    <t>3.301.624</t>
+  </si>
+  <si>
+    <t>3.080.955</t>
+  </si>
+  <si>
+    <t>2.515.454</t>
+  </si>
+  <si>
+    <t>16.089.960</t>
+  </si>
+  <si>
+    <t>17.140.354</t>
+  </si>
+  <si>
+    <t>3.258.407</t>
+  </si>
+  <si>
+    <t>3.427.196</t>
+  </si>
+  <si>
+    <t>3.424.315</t>
+  </si>
+  <si>
+    <t>2.066.176</t>
   </si>
 </sst>
 </file>
@@ -553,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="166" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1026,6 +1083,258 @@
         <v>34</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2002</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>251</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2002</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>190</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2002</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>58</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2002</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2002</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>47</v>
+      </c>
+      <c r="D38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2002</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1998</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>298</v>
+      </c>
+      <c r="D40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1998</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>198</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1998</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>47</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1998</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>47</v>
+      </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1998</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1998</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>36</v>
+      </c>
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1994</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>244</v>
+      </c>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1994</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>252</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1994</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1994</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1994</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1994</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>